<commit_message>
additional reporting, updated README and REQUIREMENTS
</commit_message>
<xml_diff>
--- a/hardware/Power consumption.xlsx
+++ b/hardware/Power consumption.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernd\Documents\Documents\Projects\HomeAutomation\MySoilSensorESP32\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5A6720-708A-4667-A1DC-CAAC1CA04643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ED7C16-DAD4-4844-A7EA-A22B5D40C37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="231" yWindow="4402" windowWidth="24915" windowHeight="14372" xr2:uid="{C5D42818-61E1-41CB-B279-D40255C4939D}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19563" windowHeight="13803" xr2:uid="{C5D42818-61E1-41CB-B279-D40255C4939D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{0B140197-1585-4AB9-8FEA-AE98B2B1082A}">
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{DA0235EB-4C0C-4C97-9A69-E73950A3A9FB}">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{A65A902B-EC15-49E4-A37E-7CE8D0607B04}">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{0B140197-1585-4AB9-8FEA-AE98B2B1082A}">
       <text>
         <r>
           <rPr>
@@ -135,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{DA0235EB-4C0C-4C97-9A69-E73950A3A9FB}">
+    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{A65A902B-EC15-49E4-A37E-7CE8D0607B04}">
       <text>
         <r>
           <rPr>
@@ -170,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F54" authorId="0" shapeId="0" xr:uid="{AC994FE4-F3AB-4E34-95F5-BFCD19FB6CE7}">
+    <comment ref="F55" authorId="0" shapeId="0" xr:uid="{AC994FE4-F3AB-4E34-95F5-BFCD19FB6CE7}">
       <text>
         <r>
           <rPr>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="37">
   <si>
     <t>State</t>
   </si>
@@ -248,9 +248,6 @@
     <t>years</t>
   </si>
   <si>
-    <t>Active, Wifi on, refresh display</t>
-  </si>
-  <si>
     <t>self discharge</t>
   </si>
   <si>
@@ -314,7 +311,16 @@
     <t>ESP32c3, 3x AAA 4.5V</t>
   </si>
   <si>
-    <t>ESP32-WROOM, 2x AAA</t>
+    <t>too short</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM, 2x AAA 3.0V</t>
+  </si>
+  <si>
+    <t>Active, Wifi on</t>
+  </si>
+  <si>
+    <t>Active, Wifi on, fresh connect</t>
   </si>
 </sst>
 </file>
@@ -325,7 +331,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +368,13 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -389,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -401,6 +414,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F643F03A-9FCE-4307-81DB-66D7872B7CDB}">
-  <dimension ref="B1:J85"/>
+  <dimension ref="B1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -730,12 +744,12 @@
     <col min="13" max="13" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -746,10 +760,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>2</v>
@@ -764,9 +778,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>800</v>
@@ -789,14 +803,20 @@
         <f>+E3*H3/(24*60*60)</f>
         <v>5.7777777777777775E-2</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>4.5</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="7">
-        <f>+C76</f>
-        <v>3.1914893617021276</v>
+        <f>+M7</f>
+        <v>4.7872340425531918</v>
       </c>
       <c r="H4">
         <f>24*60*60</f>
@@ -804,14 +824,20 @@
       </c>
       <c r="I4" s="4">
         <f>+(E4+F4/1000)*H4/3600</f>
-        <v>7.6595744680851063E-2</v>
+        <v>0.1148936170212766</v>
       </c>
       <c r="J4">
         <f>+E4*H4/(24*60*60)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>470</v>
+      </c>
+      <c r="N4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -830,10 +856,16 @@
         <f>+E5*H5/(24*60*60)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>470</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>35</v>
@@ -847,56 +879,76 @@
         <v>0.84000000000000008</v>
       </c>
       <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M6" s="4">
+        <f>+M3*M4/(M4+M5)</f>
+        <v>2.25</v>
+      </c>
+      <c r="N6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I7" s="5">
         <f>SUM(I3:I6)</f>
-        <v>2.6391130780141845</v>
+        <v>2.6774109503546102</v>
       </c>
       <c r="J7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M7" s="7">
+        <f>1000*M3/(M4+M5)</f>
+        <v>4.7872340425531918</v>
+      </c>
+      <c r="N7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I8">
         <v>1250</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I9" s="2">
         <v>0.75</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="N9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I10" s="1">
         <f>+I8*I9/I7</f>
-        <v>355.23297876475499</v>
+        <v>350.151701544297</v>
       </c>
       <c r="J10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I11" s="7">
         <f>+I10/365</f>
-        <v>0.97324103771165749</v>
+        <v>0.95931973025834794</v>
       </c>
       <c r="J11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>0</v>
       </c>
@@ -907,10 +959,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>2</v>
@@ -925,732 +977,863 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D15">
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="E15">
         <v>130</v>
       </c>
       <c r="G15">
+        <v>22</v>
+      </c>
+      <c r="H15">
+        <f>+G15*D15/1000</f>
+        <v>22</v>
+      </c>
+      <c r="I15" s="4">
+        <f>+(E15+F15/1000)*H15/3600</f>
+        <v>0.7944444444444444</v>
+      </c>
+      <c r="J15">
+        <f>+E15*H15/(24*60*60)</f>
+        <v>3.3101851851851855E-2</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+      <c r="N15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16">
+        <v>2500</v>
+      </c>
+      <c r="E16">
+        <v>130</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <f>+G16*D16/1000</f>
+        <v>5</v>
+      </c>
+      <c r="I16" s="4">
+        <f>+(E16+F16/1000)*H16/3600</f>
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="J16">
+        <f>+E16*H16/(24*60*60)</f>
+        <v>7.5231481481481477E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="7">
+        <f>+M20</f>
+        <v>3.1914893617021276</v>
+      </c>
+      <c r="H17">
+        <f>24*60*60</f>
+        <v>86400</v>
+      </c>
+      <c r="I17" s="4">
+        <f>+(E17+F17/1000)*H17/3600</f>
+        <v>7.6595744680851063E-2</v>
+      </c>
+      <c r="J17">
+        <f>+E17*H17/(24*60*60)</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>470</v>
+      </c>
+      <c r="N17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>14</v>
+      </c>
+      <c r="H18">
+        <f>24*60*60-SUM(H15:H15)</f>
+        <v>86378</v>
+      </c>
+      <c r="I18" s="4">
+        <f>+(E18+F18/1000)*H18/3600</f>
+        <v>0.3359144444444444</v>
+      </c>
+      <c r="J18" s="6">
+        <f>+E18*H18/(24*60*60)</f>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>470</v>
+      </c>
+      <c r="N18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>35</v>
+      </c>
+      <c r="H19">
+        <f>24*60*60</f>
+        <v>86400</v>
+      </c>
+      <c r="I19" s="4">
+        <f>+(E19+F19/1000)*H19/3600</f>
+        <v>0.84000000000000008</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="M19" s="4">
+        <f>+M15*M17/(M17+M18)</f>
+        <v>1.5</v>
+      </c>
+      <c r="N19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I20" s="5">
+        <f>SUM(I15:I19)</f>
+        <v>2.2275101891252955</v>
+      </c>
+      <c r="J20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M20" s="7">
+        <f>1000*M15/(M17+M18)</f>
+        <v>3.1914893617021276</v>
+      </c>
+      <c r="N20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>1250</v>
+      </c>
+      <c r="J21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I22" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="J22" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="N22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I23" s="1">
+        <f>+I21*I22/I20</f>
+        <v>420.87349569796578</v>
+      </c>
+      <c r="J23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I24" s="7">
+        <f>+I23/365</f>
+        <v>1.1530780704053858</v>
+      </c>
+      <c r="J24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28">
+        <v>800</v>
+      </c>
+      <c r="E28">
+        <v>130</v>
+      </c>
+      <c r="G28">
         <f>+G3</f>
         <v>48</v>
       </c>
-      <c r="H15">
-        <f>+G15*D15/1000</f>
+      <c r="H28">
+        <f>+G28*D28/1000</f>
         <v>38.4</v>
       </c>
-      <c r="I15" s="4">
-        <f>+(E15+F15/1000)*H15/3600</f>
+      <c r="I28" s="4">
+        <f>+(E28+F28/1000)*H28/3600</f>
         <v>1.3866666666666667</v>
       </c>
-      <c r="J15">
-        <f>+E15*H15/(24*60*60)</f>
+      <c r="J28">
+        <f>+E28*H28/(24*60*60)</f>
         <v>5.7777777777777775E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="7">
-        <f>+F4</f>
+      <c r="M28">
+        <v>3</v>
+      </c>
+      <c r="N28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="7">
+        <f>+M32</f>
         <v>3.1914893617021276</v>
       </c>
-      <c r="H16">
+      <c r="H29">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I16" s="4">
-        <f>+(E16+F16/1000)*H16/3600</f>
+      <c r="I29" s="4">
+        <f>+(E29+F29/1000)*H29/3600</f>
         <v>7.6595744680851063E-2</v>
       </c>
-      <c r="J16">
-        <f>+E16*H16/(24*60*60)</f>
+      <c r="J29">
+        <f>+E29*H29/(24*60*60)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="M29">
+        <v>470</v>
+      </c>
+      <c r="N29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>5</v>
       </c>
-      <c r="F17">
+      <c r="F30">
         <v>5</v>
       </c>
-      <c r="H17">
-        <f>24*60*60-SUM(H15:H15)</f>
+      <c r="H30">
+        <f>24*60*60-SUM(H28:H28)</f>
         <v>86361.600000000006</v>
       </c>
-      <c r="I17" s="4">
-        <f>+(E17+F17/1000)*H17/3600</f>
+      <c r="I30" s="4">
+        <f>+(E30+F30/1000)*H30/3600</f>
         <v>0.11994666666666667</v>
       </c>
-      <c r="J17" s="6">
-        <f>+E17*H17/(24*60*60)</f>
+      <c r="J30" s="6">
+        <f>+E30*H30/(24*60*60)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18">
+      <c r="M30">
+        <v>470</v>
+      </c>
+      <c r="N30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31">
         <v>80</v>
       </c>
-      <c r="H18">
+      <c r="H31">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I18" s="4">
-        <f>+(E18+F18/1000)*H18/3600</f>
+      <c r="I31" s="4">
+        <f>+(E31+F31/1000)*H31/3600</f>
         <v>1.92</v>
       </c>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I19" s="5">
-        <f>SUM(I15:I18)</f>
+      <c r="J31" s="6"/>
+      <c r="M31" s="4">
+        <f>+M28*M29/(M29+M30)</f>
+        <v>1.5</v>
+      </c>
+      <c r="N31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I32" s="5">
+        <f>SUM(I28:I31)</f>
         <v>3.5032090780141845</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J32" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I20">
+      <c r="M32" s="7">
+        <f>1000*M28/(M29+M30)</f>
+        <v>3.1914893617021276</v>
+      </c>
+      <c r="N32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I33">
         <v>2890</v>
       </c>
-      <c r="J20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I21" s="2">
+      <c r="J33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I34" s="2">
         <v>0.75</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J34" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I22" s="1">
-        <f>+I20*I21/I19</f>
+      <c r="M34">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="N34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I35" s="1">
+        <f>+I33*I34/I32</f>
         <v>618.71842408808232</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I23" s="7">
-        <f>+I22/365</f>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I36" s="7">
+        <f>+I35/365</f>
         <v>1.6951189701043352</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E39" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H39" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I39" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="J39" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27">
-        <v>800</v>
-      </c>
-      <c r="E27">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40">
+        <v>1000</v>
+      </c>
+      <c r="E40">
         <v>130</v>
       </c>
-      <c r="G27">
+      <c r="G40">
         <f>+G3</f>
         <v>48</v>
       </c>
-      <c r="H27">
-        <f>+G27*D27/1000</f>
-        <v>38.4</v>
-      </c>
-      <c r="I27" s="4">
-        <f>+(E27+F27/1000)*H27/3600</f>
-        <v>1.3866666666666667</v>
-      </c>
-      <c r="J27">
-        <f>+E27*H27/(24*60*60)</f>
-        <v>5.7777777777777775E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="7">
-        <f>+F16</f>
+      <c r="H40">
+        <f>+G40*D40/1000</f>
+        <v>48</v>
+      </c>
+      <c r="I40" s="4">
+        <f>+(E40+F40/1000)*H40/3600</f>
+        <v>1.7333333333333334</v>
+      </c>
+      <c r="J40">
+        <f>+E40*H40/(24*60*60)</f>
+        <v>7.2222222222222215E-2</v>
+      </c>
+      <c r="M40">
+        <v>3</v>
+      </c>
+      <c r="N40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="7">
+        <f>+M44</f>
         <v>3.1914893617021276</v>
       </c>
-      <c r="H28">
+      <c r="H41">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I28" s="4">
-        <f>+(E28+F28/1000)*H28/3600</f>
+      <c r="I41" s="4">
+        <f>+(E41+F41/1000)*H41/3600</f>
         <v>7.6595744680851063E-2</v>
       </c>
-      <c r="J28">
-        <f>+E28*H28/(24*60*60)</f>
+      <c r="J41">
+        <f>+E41*H41/(24*60*60)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="M41">
+        <v>470</v>
+      </c>
+      <c r="N41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>5</v>
       </c>
-      <c r="F29">
+      <c r="F42">
         <v>5</v>
       </c>
-      <c r="H29">
-        <f>24*60*60-SUM(H27:H27)</f>
-        <v>86361.600000000006</v>
-      </c>
-      <c r="I29" s="4">
-        <f>+(E29+F29/1000)*H29/3600</f>
-        <v>0.11994666666666667</v>
-      </c>
-      <c r="J29" s="6">
-        <f>+E29*H29/(24*60*60)</f>
+      <c r="H42">
+        <f>24*60*60-SUM(H40:H40)</f>
+        <v>86352</v>
+      </c>
+      <c r="I42" s="4">
+        <f>+(E42+F42/1000)*H42/3600</f>
+        <v>0.11993333333333334</v>
+      </c>
+      <c r="J42" s="6">
+        <f>+E42*H42/(24*60*60)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30">
+      <c r="M42">
+        <v>470</v>
+      </c>
+      <c r="N42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43">
         <v>3</v>
       </c>
-      <c r="H30">
+      <c r="H43">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I30" s="4">
-        <f>+(E30+F30/1000)*H30/3600</f>
+      <c r="I43" s="4">
+        <f>+(E43+F43/1000)*H43/3600</f>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I31" s="5">
-        <f>SUM(I27:I30)</f>
-        <v>1.6552090780141844</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="J43" s="6"/>
+      <c r="M43" s="4">
+        <f>+M40*M41/(M41+M42)</f>
+        <v>1.5</v>
+      </c>
+      <c r="N43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I44" s="5">
+        <f>SUM(I40:I43)</f>
+        <v>2.0018624113475179</v>
+      </c>
+      <c r="J44" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I32">
+      <c r="M44" s="7">
+        <f>1000*M40/(M41+M42)</f>
+        <v>3.1914893617021276</v>
+      </c>
+      <c r="N44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I45">
         <v>220</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I46" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="J46" t="s">
+        <v>8</v>
+      </c>
+      <c r="M46">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="N46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I47" s="1">
+        <f>+I45*I46/I44</f>
+        <v>82.423247004739551</v>
+      </c>
+      <c r="J47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I48" s="7">
+        <f>+I47/365</f>
+        <v>0.22581711508147823</v>
+      </c>
+      <c r="J48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52">
+        <v>1000</v>
+      </c>
+      <c r="E52">
+        <v>20</v>
+      </c>
+      <c r="G52">
+        <f>+G40</f>
+        <v>48</v>
+      </c>
+      <c r="H52">
+        <f>+G52*D52/1000</f>
+        <v>48</v>
+      </c>
+      <c r="I52" s="4">
+        <f>+(E52+F52/1000)*H52/3600</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="J52">
+        <f>+E52*H52/(24*60*60)</f>
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="M52">
+        <v>4.5</v>
+      </c>
+      <c r="N52" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I33" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="J33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I34" s="1">
-        <f>+I32*I33/I31</f>
-        <v>99.685291841171278</v>
-      </c>
-      <c r="J34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I35" s="7">
-        <f>+I34/365</f>
-        <v>0.27311038860594872</v>
-      </c>
-      <c r="J35" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39">
-        <v>1000</v>
-      </c>
-      <c r="E39">
-        <v>130</v>
-      </c>
-      <c r="G39">
-        <v>24</v>
-      </c>
-      <c r="H39">
-        <f>+G39*D39/1000</f>
-        <v>24</v>
-      </c>
-      <c r="I39" s="4">
-        <f>+(E39+F39/1000)*H39/3600</f>
-        <v>0.8666666666666667</v>
-      </c>
-      <c r="J39">
-        <f>+E39*H39/(24*60*60)</f>
-        <v>3.6111111111111108E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F40" s="7">
-        <f>+F28</f>
-        <v>3.1914893617021276</v>
-      </c>
-      <c r="H40">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="7">
+        <f>+M56</f>
+        <v>4.7872340425531918</v>
+      </c>
+      <c r="H53">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I40" s="4">
-        <f>+(E40+F40/1000)*H40/3600</f>
-        <v>7.6595744680851063E-2</v>
-      </c>
-      <c r="J40">
-        <f>+E40*H40/(24*60*60)</f>
+      <c r="I53" s="4">
+        <f>+(E53+F53/1000)*H53/3600</f>
+        <v>0.1148936170212766</v>
+      </c>
+      <c r="J53">
+        <f>+E53*H53/(24*60*60)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="M53">
+        <v>470</v>
+      </c>
+      <c r="N53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>5</v>
       </c>
-      <c r="F41">
-        <v>14</v>
-      </c>
-      <c r="H41">
-        <f>24*60*60-SUM(H39:H39)</f>
-        <v>86376</v>
-      </c>
-      <c r="I41" s="4">
-        <f>+(E41+F41/1000)*H41/3600</f>
-        <v>0.33590666666666669</v>
-      </c>
-      <c r="J41" s="6">
-        <f>+E41*H41/(24*60*60)</f>
+      <c r="F54">
+        <v>40</v>
+      </c>
+      <c r="H54">
+        <f>24*60*60-SUM(H52:H52)</f>
+        <v>86352</v>
+      </c>
+      <c r="I54" s="4">
+        <f>+(E54+F54/1000)*H54/3600</f>
+        <v>0.95946666666666669</v>
+      </c>
+      <c r="J54" s="6">
+        <f>+E54*H54/(24*60*60)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42">
+      <c r="M54">
+        <v>470</v>
+      </c>
+      <c r="N54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55">
         <v>35</v>
       </c>
-      <c r="H42">
+      <c r="H55">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I42" s="4">
-        <f>+(E42+F42/1000)*H42/3600</f>
+      <c r="I55" s="4">
+        <f>+(E55+F55/1000)*H55/3600</f>
         <v>0.84000000000000008</v>
       </c>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I43" s="5">
-        <f>SUM(I39:I42)</f>
-        <v>2.1191690780141847</v>
-      </c>
-      <c r="J43" t="s">
+      <c r="J55" s="6"/>
+      <c r="M55" s="4">
+        <f>+M52*M53/(M53+M54)</f>
+        <v>2.25</v>
+      </c>
+      <c r="N55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I56" s="5">
+        <f>SUM(I52:I55)</f>
+        <v>2.1810269503546102</v>
+      </c>
+      <c r="J56" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I44">
+      <c r="M56" s="7">
+        <f>1000*M52/(M53+M54)</f>
+        <v>4.7872340425531918</v>
+      </c>
+      <c r="N56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I57">
         <v>1250</v>
       </c>
-      <c r="J44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I45" s="2">
+      <c r="J57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I58" s="2">
         <v>0.75</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J58" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I46" s="1">
-        <f>+I44*I45/I43</f>
-        <v>442.39037353192487</v>
-      </c>
-      <c r="J46" t="s">
+      <c r="M58">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="N58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I59" s="1">
+        <f>+I57*I58/I56</f>
+        <v>429.84338173701758</v>
+      </c>
+      <c r="J59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I47" s="7">
-        <f>+I46/365</f>
-        <v>1.2120284206354106</v>
-      </c>
-      <c r="J47" t="s">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I60" s="7">
+        <f>+I59/365</f>
+        <v>1.1776531006493631</v>
+      </c>
+      <c r="J60" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>12</v>
-      </c>
-      <c r="D51">
-        <v>800</v>
-      </c>
-      <c r="E51">
+    <row r="67" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <v>4.2</v>
+      </c>
+      <c r="J67" t="s">
         <v>20</v>
       </c>
-      <c r="G51">
-        <f>+G27</f>
-        <v>48</v>
-      </c>
-      <c r="H51">
-        <f>+G51*D51/1000</f>
-        <v>38.4</v>
-      </c>
-      <c r="I51" s="4">
-        <f>+(E51+F51/1000)*H51/3600</f>
-        <v>0.21333333333333335</v>
-      </c>
-      <c r="J51">
-        <f>+E51*H51/(24*60*60)</f>
-        <v>8.8888888888888889E-3</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>26</v>
-      </c>
-      <c r="F52" s="7">
-        <f>+F28</f>
-        <v>3.1914893617021276</v>
-      </c>
-      <c r="H52">
-        <f>24*60*60</f>
-        <v>86400</v>
-      </c>
-      <c r="I52" s="4">
-        <f>+(E52+F52/1000)*H52/3600</f>
-        <v>7.6595744680851063E-2</v>
-      </c>
-      <c r="J52">
-        <f>+E52*H52/(24*60*60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>5</v>
-      </c>
-      <c r="F53">
-        <v>40</v>
-      </c>
-      <c r="H53">
-        <f>24*60*60-SUM(H51:H51)</f>
-        <v>86361.600000000006</v>
-      </c>
-      <c r="I53" s="4">
-        <f>+(E53+F53/1000)*H53/3600</f>
-        <v>0.95957333333333339</v>
-      </c>
-      <c r="J53" s="6">
-        <f>+E53*H53/(24*60*60)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54">
-        <v>35</v>
-      </c>
-      <c r="H54">
-        <f>24*60*60</f>
-        <v>86400</v>
-      </c>
-      <c r="I54" s="4">
-        <f>+(E54+F54/1000)*H54/3600</f>
-        <v>0.84000000000000008</v>
-      </c>
-      <c r="J54" s="6"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I55" s="5">
-        <f>SUM(I51:I54)</f>
-        <v>2.0895024113475182</v>
-      </c>
-      <c r="J55" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I56">
-        <v>1250</v>
-      </c>
-      <c r="J56" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I57" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="J57" t="s">
+    </row>
+    <row r="68" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I68" s="7">
+        <f>+I7*I67</f>
+        <v>11.245125991489363</v>
+      </c>
+      <c r="J68" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I69">
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I58" s="1">
-        <f>+I56*I57/I55</f>
-        <v>448.67141330332663</v>
-      </c>
-      <c r="J58" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I59" s="7">
-        <f>+I58/365</f>
-        <v>1.2292367487762375</v>
-      </c>
-      <c r="J59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I66">
-        <v>4.2</v>
-      </c>
-      <c r="J66" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I67" s="7">
-        <f>+I7*I66</f>
-        <v>11.084274927659575</v>
-      </c>
-      <c r="J67" t="s">
+      <c r="J69" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I68">
-        <v>8</v>
-      </c>
-      <c r="J68" t="s">
+    <row r="70" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I70" s="7">
+        <f>+I68/I69</f>
+        <v>1.4056407489361704</v>
+      </c>
+      <c r="J70" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I69" s="7">
-        <f>+I67/I68</f>
-        <v>1.3855343659574468</v>
-      </c>
-      <c r="J69" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="72" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C72">
-        <v>3</v>
-      </c>
-      <c r="D72" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="73" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C73">
-        <v>470</v>
-      </c>
-      <c r="D73" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="74" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C74">
-        <v>470</v>
-      </c>
-      <c r="D74" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C75" s="4">
-        <f>+C72*C73/(C73+C74)</f>
-        <v>1.5</v>
-      </c>
-      <c r="D75" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C76" s="7">
-        <f>1000*C72/(C73+C74)</f>
-        <v>3.1914893617021276</v>
-      </c>
-      <c r="D76" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C78">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="D78" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C82">
-        <v>1</v>
       </c>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C83">
-        <v>2555</v>
-      </c>
-      <c r="D83" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C84">
-        <f>+C73/(C73+C74)</f>
-        <v>0.5</v>
+        <v>2555</v>
       </c>
       <c r="D84" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C85">
-        <f>+C83*C82/C84</f>
+        <f>+M53/(M53+M54)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D85" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <f>+C84*C83/C85</f>
         <v>5110</v>
       </c>
-      <c r="D85" t="s">
-        <v>29</v>
+      <c r="D86" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
measurements *before* turning on WiFi, and general cleanup
</commit_message>
<xml_diff>
--- a/hardware/Power consumption.xlsx
+++ b/hardware/Power consumption.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernd\Documents\Documents\Projects\HomeAutomation\MySoilSensorESP32\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E1868F-B541-463B-A031-E57284DE4359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD77832-1922-41EC-BB72-C4EFA4B95B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9428" yWindow="3478" windowWidth="23665" windowHeight="14373" xr2:uid="{C5D42818-61E1-41CB-B279-D40255C4939D}"/>
+    <workbookView xWindow="3043" yWindow="3043" windowWidth="21682" windowHeight="14373" xr2:uid="{C5D42818-61E1-41CB-B279-D40255C4939D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>bernd</author>
   </authors>
   <commentList>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{B44EB038-C6AC-4BFE-A03F-74DCCADF4C25}">
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{B44EB038-C6AC-4BFE-A03F-74DCCADF4C25}">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{DA0235EB-4C0C-4C97-9A69-E73950A3A9FB}">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{DA0235EB-4C0C-4C97-9A69-E73950A3A9FB}">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{0B140197-1585-4AB9-8FEA-AE98B2B1082A}">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{0B140197-1585-4AB9-8FEA-AE98B2B1082A}">
       <text>
         <r>
           <rPr>
@@ -135,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{A65A902B-EC15-49E4-A37E-7CE8D0607B04}">
+    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{A65A902B-EC15-49E4-A37E-7CE8D0607B04}">
       <text>
         <r>
           <rPr>
@@ -170,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F55" authorId="0" shapeId="0" xr:uid="{AC994FE4-F3AB-4E34-95F5-BFCD19FB6CE7}">
+    <comment ref="F58" authorId="0" shapeId="0" xr:uid="{AC994FE4-F3AB-4E34-95F5-BFCD19FB6CE7}">
       <text>
         <r>
           <rPr>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="42">
   <si>
     <t>State</t>
   </si>
@@ -320,7 +320,22 @@
     <t>Active, Wifi on</t>
   </si>
   <si>
-    <t>Active, Wifi on, fresh connect</t>
+    <t>V supply</t>
+  </si>
+  <si>
+    <t>kOhm pulldown</t>
+  </si>
+  <si>
+    <t>µA current per channel</t>
+  </si>
+  <si>
+    <t>channels</t>
+  </si>
+  <si>
+    <t>µA current total</t>
+  </si>
+  <si>
+    <t>Active, Wifi off</t>
   </si>
 </sst>
 </file>
@@ -729,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F643F03A-9FCE-4307-81DB-66D7872B7CDB}">
-  <dimension ref="B1:N86"/>
+  <dimension ref="B1:R89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:I16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -744,12 +759,12 @@
     <col min="13" max="13" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -778,30 +793,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D3">
-        <v>800</v>
+        <v>300</v>
       </c>
       <c r="E3">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="G3">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="H3">
         <f>+G3*D3/1000</f>
-        <v>38.4</v>
+        <v>7.2</v>
       </c>
       <c r="I3" s="4">
         <f>+(E3+F3/1000)*H3/3600</f>
-        <v>1.3866666666666667</v>
+        <v>0.1</v>
       </c>
       <c r="J3">
         <f>+E3*H3/(24*60*60)</f>
-        <v>5.7777777777777775E-2</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="M3">
         <v>4.5</v>
@@ -809,50 +824,62 @@
       <c r="N3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>3</v>
+      </c>
+      <c r="R3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4">
+        <v>300</v>
+      </c>
+      <c r="E4">
+        <v>130</v>
+      </c>
+      <c r="G4">
+        <v>24</v>
+      </c>
+      <c r="H4">
+        <f>+G4*D4/1000</f>
+        <v>7.2</v>
+      </c>
+      <c r="I4" s="4">
+        <f>+(E4+F4/1000)*H4/3600</f>
+        <v>0.26</v>
+      </c>
+      <c r="J4">
+        <f>+E4*H4/(24*60*60)</f>
+        <v>1.0833333333333334E-2</v>
+      </c>
+      <c r="Q4">
+        <v>200</v>
+      </c>
+      <c r="R4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="7">
-        <f>+M7</f>
+      <c r="F5" s="7">
+        <f>+M8</f>
         <v>4.7872340425531918</v>
       </c>
-      <c r="H4">
+      <c r="H5">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I4" s="4">
-        <f>+(E4+F4/1000)*H4/3600</f>
-        <v>0.1148936170212766</v>
-      </c>
-      <c r="J4">
-        <f>+E4*H4/(24*60*60)</f>
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>470</v>
-      </c>
-      <c r="N4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>14</v>
-      </c>
-      <c r="H5">
-        <f>24*60*60-SUM(H3:H3)</f>
-        <v>86361.600000000006</v>
-      </c>
       <c r="I5" s="4">
         <f>+(E5+F5/1000)*H5/3600</f>
-        <v>0.33585066666666669</v>
-      </c>
-      <c r="J5" s="6">
+        <v>0.1148936170212766</v>
+      </c>
+      <c r="J5">
         <f>+E5*H5/(24*60*60)</f>
         <v>0</v>
       </c>
@@ -862,222 +889,242 @@
       <c r="N5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <f>1000*Q3/Q4</f>
+        <v>15</v>
+      </c>
+      <c r="R5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <f>24*60*60-SUM(H3:H3)</f>
+        <v>86392.8</v>
+      </c>
+      <c r="I6" s="4">
+        <f>+(E6+F6/1000)*H6/3600</f>
+        <v>0.33597199999999999</v>
+      </c>
+      <c r="J6" s="6">
+        <f>+E6*H6/(24*60*60)</f>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>470</v>
+      </c>
+      <c r="N6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>35</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I6" s="4">
-        <f>+(E6+F6/1000)*H6/3600</f>
+      <c r="I7" s="4">
+        <f>+(E7+F7/1000)*H7/3600</f>
         <v>0.84000000000000008</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="M6" s="4">
-        <f>+M3*M4/(M4+M5)</f>
+      <c r="J7" s="6"/>
+      <c r="M7" s="4">
+        <f>+M3*M5/(M5+M6)</f>
         <v>2.25</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I7" s="5">
-        <f>SUM(I3:I6)</f>
-        <v>2.6774109503546102</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="Q7">
+        <f>+Q5*Q6</f>
+        <v>60</v>
+      </c>
+      <c r="R7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="I8" s="5">
+        <f>SUM(I3:I7)</f>
+        <v>1.6508656170212768</v>
+      </c>
+      <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="7">
-        <f>1000*M3/(M4+M5)</f>
+      <c r="M8" s="7">
+        <f>1000*M3/(M5+M6)</f>
         <v>4.7872340425531918</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I8">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="I9">
         <v>1250</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I9" s="2">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
         <v>0.75</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>8</v>
       </c>
-      <c r="M9">
+      <c r="M10">
         <v>2.4500000000000002</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I10" s="1">
-        <f>+I8*I9/I7</f>
-        <v>350.151701544297</v>
-      </c>
-      <c r="J10" t="s">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="I11" s="1">
+        <f>+I9*I10/I8</f>
+        <v>567.88389698948902</v>
+      </c>
+      <c r="J11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I11" s="7">
-        <f>+I10/365</f>
-        <v>0.95931973025834794</v>
-      </c>
-      <c r="J11" t="s">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="I12" s="7">
+        <f>+I11/365</f>
+        <v>1.5558462931218877</v>
+      </c>
+      <c r="J12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+    <row r="15" spans="2:18" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15">
-        <v>400</v>
-      </c>
-      <c r="E15">
-        <v>130</v>
-      </c>
-      <c r="G15">
-        <v>22</v>
-      </c>
-      <c r="H15">
-        <f>+G15*D15/1000</f>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="I15" s="4">
-        <f>+(E15+F15/1000)*H15/3600</f>
-        <v>0.31777777777777777</v>
-      </c>
-      <c r="J15">
-        <f>+E15*H15/(24*60*60)</f>
-        <v>1.324074074074074E-2</v>
-      </c>
-      <c r="M15">
-        <v>3</v>
-      </c>
-      <c r="N15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D16">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="E16">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="H16">
         <f>+G16*D16/1000</f>
-        <v>2</v>
+        <v>7.2</v>
       </c>
       <c r="I16" s="4">
         <f>+(E16+F16/1000)*H16/3600</f>
-        <v>7.2222222222222215E-2</v>
+        <v>0.1</v>
       </c>
       <c r="J16">
         <f>+E16*H16/(24*60*60)</f>
-        <v>3.0092592592592593E-3</v>
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <v>300</v>
+      </c>
+      <c r="E17">
+        <v>130</v>
+      </c>
+      <c r="G17">
+        <v>24</v>
+      </c>
+      <c r="H17">
+        <f>+G17*D17/1000</f>
+        <v>7.2</v>
+      </c>
+      <c r="I17" s="4">
+        <f>+(E17+F17/1000)*H17/3600</f>
+        <v>0.26</v>
+      </c>
+      <c r="J17">
+        <f>+E17*H17/(24*60*60)</f>
+        <v>1.0833333333333334E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="7">
-        <f>+M20</f>
+      <c r="F18" s="7">
+        <f>+M21</f>
         <v>3.1914893617021276</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I17" s="4">
-        <f>+(E17+F17/1000)*H17/3600</f>
-        <v>7.6595744680851063E-2</v>
-      </c>
-      <c r="J17">
-        <f>+E17*H17/(24*60*60)</f>
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>470</v>
-      </c>
-      <c r="N17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18">
-        <v>14</v>
-      </c>
-      <c r="H18">
-        <f>24*60*60-SUM(H15:H15)</f>
-        <v>86391.2</v>
-      </c>
       <c r="I18" s="4">
         <f>+(E18+F18/1000)*H18/3600</f>
-        <v>0.33596577777777775</v>
-      </c>
-      <c r="J18" s="6">
+        <v>7.6595744680851063E-2</v>
+      </c>
+      <c r="J18">
         <f>+E18*H18/(24*60*60)</f>
         <v>0</v>
       </c>
@@ -1090,210 +1137,209 @@
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>14</v>
+      </c>
+      <c r="H19">
+        <f>24*60*60-SUM(H16:H16)</f>
+        <v>86392.8</v>
+      </c>
+      <c r="I19" s="4">
+        <f>+(E19+F19/1000)*H19/3600</f>
+        <v>0.33597199999999999</v>
+      </c>
+      <c r="J19" s="6">
+        <f>+E19*H19/(24*60*60)</f>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>470</v>
+      </c>
+      <c r="N19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>12</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>35</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I19" s="4">
-        <f>+(E19+F19/1000)*H19/3600</f>
+      <c r="I20" s="4">
+        <f>+(E20+F20/1000)*H20/3600</f>
         <v>0.84000000000000008</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="M19" s="4">
-        <f>+M15*M17/(M17+M18)</f>
+      <c r="J20" s="6"/>
+      <c r="M20" s="4">
+        <f>+M16*M18/(M18+M19)</f>
         <v>1.5</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I20" s="5">
-        <f>SUM(I15:I19)</f>
-        <v>1.642561522458629</v>
-      </c>
-      <c r="J20" t="s">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I21" s="5">
+        <f>SUM(I16:I20)</f>
+        <v>1.6125677446808511</v>
+      </c>
+      <c r="J21" t="s">
         <v>6</v>
       </c>
-      <c r="M20" s="7">
-        <f>1000*M15/(M17+M18)</f>
+      <c r="M21" s="7">
+        <f>1000*M16/(M18+M19)</f>
         <v>3.1914893617021276</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I21">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I22">
         <v>1250</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I22" s="2">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I23" s="2">
         <v>0.75</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J23" t="s">
         <v>8</v>
       </c>
-      <c r="M22">
+      <c r="M23">
         <v>2.4500000000000002</v>
       </c>
-      <c r="N22" t="s">
+      <c r="N23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I23" s="1">
-        <f>+I21*I22/I20</f>
-        <v>570.75487717301792</v>
-      </c>
-      <c r="J23" t="s">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I24" s="1">
+        <f>+I22*I23/I21</f>
+        <v>581.3709241626583</v>
+      </c>
+      <c r="J24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I24" s="7">
-        <f>+I23/365</f>
-        <v>1.5637119922548437</v>
-      </c>
-      <c r="J24" t="s">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I25" s="7">
+        <f>+I24/365</f>
+        <v>1.5927970525004338</v>
+      </c>
+      <c r="J25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+    <row r="28" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28">
-        <v>800</v>
-      </c>
-      <c r="E28">
-        <v>130</v>
-      </c>
-      <c r="G28">
-        <f>+G3</f>
-        <v>48</v>
-      </c>
-      <c r="H28">
-        <f>+G28*D28/1000</f>
-        <v>38.4</v>
-      </c>
-      <c r="I28" s="4">
-        <f>+(E28+F28/1000)*H28/3600</f>
-        <v>1.3866666666666667</v>
-      </c>
-      <c r="J28">
-        <f>+E28*H28/(24*60*60)</f>
-        <v>5.7777777777777775E-2</v>
-      </c>
-      <c r="M28">
-        <v>3</v>
-      </c>
-      <c r="N28" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="7">
-        <f>+M32</f>
-        <v>3.1914893617021276</v>
+        <v>41</v>
+      </c>
+      <c r="D29">
+        <v>300</v>
+      </c>
+      <c r="E29">
+        <v>50</v>
+      </c>
+      <c r="G29">
+        <v>24</v>
       </c>
       <c r="H29">
-        <f>24*60*60</f>
-        <v>86400</v>
+        <f>+G29*D29/1000</f>
+        <v>7.2</v>
       </c>
       <c r="I29" s="4">
         <f>+(E29+F29/1000)*H29/3600</f>
-        <v>7.6595744680851063E-2</v>
+        <v>0.1</v>
       </c>
       <c r="J29">
         <f>+E29*H29/(24*60*60)</f>
-        <v>0</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="M29">
-        <v>470</v>
+        <v>3</v>
       </c>
       <c r="N29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="D30">
+        <v>300</v>
+      </c>
+      <c r="E30">
+        <v>130</v>
+      </c>
+      <c r="G30">
+        <v>24</v>
       </c>
       <c r="H30">
-        <f>24*60*60-SUM(H28:H28)</f>
-        <v>86361.600000000006</v>
+        <f>+G30*D30/1000</f>
+        <v>7.2</v>
       </c>
       <c r="I30" s="4">
         <f>+(E30+F30/1000)*H30/3600</f>
-        <v>0.11994666666666667</v>
-      </c>
-      <c r="J30" s="6">
+        <v>0.26</v>
+      </c>
+      <c r="J30">
         <f>+E30*H30/(24*60*60)</f>
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>470</v>
-      </c>
-      <c r="N30" t="s">
-        <v>17</v>
+        <v>1.0833333333333334E-2</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31">
-        <v>80</v>
+        <v>25</v>
+      </c>
+      <c r="F31" s="7">
+        <f>+M34</f>
+        <v>3.1914893617021276</v>
       </c>
       <c r="H31">
         <f>24*60*60</f>
@@ -1301,538 +1347,615 @@
       </c>
       <c r="I31" s="4">
         <f>+(E31+F31/1000)*H31/3600</f>
-        <v>1.92</v>
-      </c>
-      <c r="J31" s="6"/>
-      <c r="M31" s="4">
-        <f>+M28*M29/(M29+M30)</f>
-        <v>1.5</v>
+        <v>7.6595744680851063E-2</v>
+      </c>
+      <c r="J31">
+        <f>+E31*H31/(24*60*60)</f>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>470</v>
       </c>
       <c r="N31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I32" s="5">
-        <f>SUM(I28:I31)</f>
-        <v>3.5032090780141845</v>
-      </c>
-      <c r="J32" t="s">
-        <v>6</v>
-      </c>
-      <c r="M32" s="7">
-        <f>1000*M28/(M29+M30)</f>
-        <v>3.1914893617021276</v>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>5</v>
+      </c>
+      <c r="H32">
+        <f>24*60*60-SUM(H29:H29)</f>
+        <v>86392.8</v>
+      </c>
+      <c r="I32" s="4">
+        <f>+(E32+F32/1000)*H32/3600</f>
+        <v>0.11999</v>
+      </c>
+      <c r="J32" s="6">
+        <f>+E32*H32/(24*60*60)</f>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>470</v>
       </c>
       <c r="N32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I33">
-        <v>2890</v>
-      </c>
-      <c r="J33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I34" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="J34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M34">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="N34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I35" s="1">
-        <f>+I33*I34/I32</f>
-        <v>618.71842408808232</v>
-      </c>
-      <c r="J35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I36" s="7">
-        <f>+I35/365</f>
-        <v>1.6951189701043352</v>
-      </c>
-      <c r="J36" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40">
-        <v>1000</v>
-      </c>
-      <c r="E40">
-        <v>130</v>
-      </c>
-      <c r="G40">
-        <f>+G3</f>
-        <v>48</v>
-      </c>
-      <c r="H40">
-        <f>+G40*D40/1000</f>
-        <v>48</v>
-      </c>
-      <c r="I40" s="4">
-        <f>+(E40+F40/1000)*H40/3600</f>
-        <v>1.7333333333333334</v>
-      </c>
-      <c r="J40">
-        <f>+E40*H40/(24*60*60)</f>
-        <v>7.2222222222222215E-2</v>
-      </c>
-      <c r="M40">
-        <v>3</v>
-      </c>
-      <c r="N40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="7">
-        <f>+M44</f>
-        <v>3.1914893617021276</v>
-      </c>
-      <c r="H41">
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33">
+        <v>80</v>
+      </c>
+      <c r="H33">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I41" s="4">
-        <f>+(E41+F41/1000)*H41/3600</f>
-        <v>7.6595744680851063E-2</v>
-      </c>
-      <c r="J41">
-        <f>+E41*H41/(24*60*60)</f>
+      <c r="I33" s="4">
+        <f>+(E33+F33/1000)*H33/3600</f>
+        <v>1.92</v>
+      </c>
+      <c r="J33" s="6"/>
+      <c r="M33" s="4">
+        <f>+M29*M31/(M31+M32)</f>
+        <v>1.5</v>
+      </c>
+      <c r="N33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I34" s="5">
+        <f>SUM(I29:I33)</f>
+        <v>2.4765857446808512</v>
+      </c>
+      <c r="J34" t="s">
+        <v>6</v>
+      </c>
+      <c r="M34" s="7">
+        <f>1000*M29/(M31+M32)</f>
+        <v>3.1914893617021276</v>
+      </c>
+      <c r="N34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>2890</v>
+      </c>
+      <c r="J35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I36" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="J36" t="s">
+        <v>8</v>
+      </c>
+      <c r="M36">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="N36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I37" s="1">
+        <f>+I35*I36/I34</f>
+        <v>875.19683283944528</v>
+      </c>
+      <c r="J37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I38" s="7">
+        <f>+I37/365</f>
+        <v>2.3977995420258775</v>
+      </c>
+      <c r="J38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M41">
-        <v>470</v>
-      </c>
-      <c r="N41" t="s">
-        <v>17</v>
+      <c r="C41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42">
-        <v>5</v>
+        <v>41</v>
+      </c>
+      <c r="D42">
+        <v>300</v>
+      </c>
+      <c r="E42">
+        <v>50</v>
+      </c>
+      <c r="G42">
+        <v>24</v>
       </c>
       <c r="H42">
-        <f>24*60*60-SUM(H40:H40)</f>
-        <v>86352</v>
+        <f>+G42*D42/1000</f>
+        <v>7.2</v>
       </c>
       <c r="I42" s="4">
         <f>+(E42+F42/1000)*H42/3600</f>
-        <v>0.11993333333333334</v>
-      </c>
-      <c r="J42" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J42">
         <f>+E42*H42/(24*60*60)</f>
-        <v>0</v>
+        <v>4.1666666666666666E-3</v>
       </c>
       <c r="M42">
-        <v>470</v>
+        <v>3</v>
       </c>
       <c r="N42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43">
-        <v>3</v>
+        <v>35</v>
+      </c>
+      <c r="D43">
+        <v>300</v>
+      </c>
+      <c r="E43">
+        <v>130</v>
+      </c>
+      <c r="G43">
+        <v>24</v>
       </c>
       <c r="H43">
+        <f>+G43*D43/1000</f>
+        <v>7.2</v>
+      </c>
+      <c r="I43" s="4">
+        <f>+(E43+F43/1000)*H43/3600</f>
+        <v>0.26</v>
+      </c>
+      <c r="J43">
+        <f>+E43*H43/(24*60*60)</f>
+        <v>1.0833333333333334E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="7">
+        <f>+M47</f>
+        <v>3.1914893617021276</v>
+      </c>
+      <c r="H44">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I43" s="4">
-        <f>+(E43+F43/1000)*H43/3600</f>
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="J43" s="6"/>
-      <c r="M43" s="4">
-        <f>+M40*M41/(M41+M42)</f>
-        <v>1.5</v>
-      </c>
-      <c r="N43" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I44" s="5">
-        <f>SUM(I40:I43)</f>
-        <v>2.0018624113475179</v>
-      </c>
-      <c r="J44" t="s">
-        <v>6</v>
-      </c>
-      <c r="M44" s="7">
-        <f>1000*M40/(M41+M42)</f>
-        <v>3.1914893617021276</v>
+      <c r="I44" s="4">
+        <f>+(E44+F44/1000)*H44/3600</f>
+        <v>7.6595744680851063E-2</v>
+      </c>
+      <c r="J44">
+        <f>+E44*H44/(24*60*60)</f>
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>470</v>
       </c>
       <c r="N44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I45">
-        <v>220</v>
-      </c>
-      <c r="J45" t="s">
-        <v>15</v>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>5</v>
+      </c>
+      <c r="H45">
+        <f>24*60*60-SUM(H42:H42)</f>
+        <v>86392.8</v>
+      </c>
+      <c r="I45" s="4">
+        <f>+(E45+F45/1000)*H45/3600</f>
+        <v>0.11999</v>
+      </c>
+      <c r="J45" s="6">
+        <f>+E45*H45/(24*60*60)</f>
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>470</v>
+      </c>
+      <c r="N45" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I46" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="J46" t="s">
-        <v>8</v>
-      </c>
-      <c r="M46">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="N46" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I47" s="1">
-        <f>+I45*I46/I44</f>
-        <v>82.423247004739551</v>
-      </c>
-      <c r="J47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I48" s="7">
-        <f>+I47/365</f>
-        <v>0.22581711508147823</v>
-      </c>
-      <c r="J48" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B50" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B51" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H51" s="3" t="s">
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46">
         <v>3</v>
       </c>
-      <c r="I51" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>35</v>
-      </c>
-      <c r="D52">
-        <v>1000</v>
-      </c>
-      <c r="E52">
-        <v>20</v>
-      </c>
-      <c r="G52">
-        <f>+G40</f>
-        <v>48</v>
-      </c>
-      <c r="H52">
-        <f>+G52*D52/1000</f>
-        <v>48</v>
-      </c>
-      <c r="I52" s="4">
-        <f>+(E52+F52/1000)*H52/3600</f>
-        <v>0.26666666666666666</v>
-      </c>
-      <c r="J52">
-        <f>+E52*H52/(24*60*60)</f>
-        <v>1.1111111111111112E-2</v>
-      </c>
-      <c r="M52">
-        <v>4.5</v>
-      </c>
-      <c r="N52" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>25</v>
-      </c>
-      <c r="F53" s="7">
-        <f>+M56</f>
-        <v>4.7872340425531918</v>
-      </c>
-      <c r="H53">
+      <c r="H46">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I53" s="4">
-        <f>+(E53+F53/1000)*H53/3600</f>
-        <v>0.1148936170212766</v>
-      </c>
-      <c r="J53">
-        <f>+E53*H53/(24*60*60)</f>
+      <c r="I46" s="4">
+        <f>+(E46+F46/1000)*H46/3600</f>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="J46" s="6"/>
+      <c r="M46" s="4">
+        <f>+M42*M44/(M44+M45)</f>
+        <v>1.5</v>
+      </c>
+      <c r="N46" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I47" s="5">
+        <f>SUM(I42:I46)</f>
+        <v>0.62858574468085104</v>
+      </c>
+      <c r="J47" t="s">
+        <v>6</v>
+      </c>
+      <c r="M47" s="7">
+        <f>1000*M42/(M44+M45)</f>
+        <v>3.1914893617021276</v>
+      </c>
+      <c r="N47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>220</v>
+      </c>
+      <c r="J48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I49" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="J49" t="s">
+        <v>8</v>
+      </c>
+      <c r="M49">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="N49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I50" s="1">
+        <f>+I48*I49/I47</f>
+        <v>262.49402153364883</v>
+      </c>
+      <c r="J50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I51" s="7">
+        <f>+I50/365</f>
+        <v>0.71916170283191461</v>
+      </c>
+      <c r="J51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B53" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M53">
-        <v>470</v>
-      </c>
-      <c r="N53" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>5</v>
-      </c>
-      <c r="F54">
-        <v>40</v>
-      </c>
-      <c r="H54">
-        <f>24*60*60-SUM(H52:H52)</f>
-        <v>86352</v>
-      </c>
-      <c r="I54" s="4">
-        <f>+(E54+F54/1000)*H54/3600</f>
-        <v>0.95946666666666669</v>
-      </c>
-      <c r="J54" s="6">
-        <f>+E54*H54/(24*60*60)</f>
-        <v>0</v>
-      </c>
-      <c r="M54">
-        <v>470</v>
-      </c>
-      <c r="N54" t="s">
-        <v>17</v>
+      <c r="C54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>12</v>
-      </c>
-      <c r="F55">
         <v>35</v>
       </c>
+      <c r="D55">
+        <v>1000</v>
+      </c>
+      <c r="E55">
+        <v>20</v>
+      </c>
+      <c r="G55">
+        <f>+G42</f>
+        <v>24</v>
+      </c>
       <c r="H55">
+        <f>+G55*D55/1000</f>
+        <v>24</v>
+      </c>
+      <c r="I55" s="4">
+        <f>+(E55+F55/1000)*H55/3600</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="J55">
+        <f>+E55*H55/(24*60*60)</f>
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="M55">
+        <v>4.5</v>
+      </c>
+      <c r="N55" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" s="7">
+        <f>+M59</f>
+        <v>4.7872340425531918</v>
+      </c>
+      <c r="H56">
         <f>24*60*60</f>
         <v>86400</v>
       </c>
-      <c r="I55" s="4">
-        <f>+(E55+F55/1000)*H55/3600</f>
+      <c r="I56" s="4">
+        <f>+(E56+F56/1000)*H56/3600</f>
+        <v>0.1148936170212766</v>
+      </c>
+      <c r="J56">
+        <f>+E56*H56/(24*60*60)</f>
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>470</v>
+      </c>
+      <c r="N56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="F57">
+        <v>40</v>
+      </c>
+      <c r="H57">
+        <f>24*60*60-SUM(H55:H55)</f>
+        <v>86376</v>
+      </c>
+      <c r="I57" s="4">
+        <f>+(E57+F57/1000)*H57/3600</f>
+        <v>0.95973333333333333</v>
+      </c>
+      <c r="J57" s="6">
+        <f>+E57*H57/(24*60*60)</f>
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>470</v>
+      </c>
+      <c r="N57" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58">
+        <v>35</v>
+      </c>
+      <c r="H58">
+        <f>24*60*60</f>
+        <v>86400</v>
+      </c>
+      <c r="I58" s="4">
+        <f>+(E58+F58/1000)*H58/3600</f>
         <v>0.84000000000000008</v>
       </c>
-      <c r="J55" s="6"/>
-      <c r="M55" s="4">
-        <f>+M52*M53/(M53+M54)</f>
+      <c r="J58" s="6"/>
+      <c r="M58" s="4">
+        <f>+M55*M56/(M56+M57)</f>
         <v>2.25</v>
       </c>
-      <c r="N55" t="s">
+      <c r="N58" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I56" s="5">
-        <f>SUM(I52:I55)</f>
-        <v>2.1810269503546102</v>
-      </c>
-      <c r="J56" t="s">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I59" s="5">
+        <f>SUM(I55:I58)</f>
+        <v>2.0479602836879431</v>
+      </c>
+      <c r="J59" t="s">
         <v>6</v>
       </c>
-      <c r="M56" s="7">
-        <f>1000*M52/(M53+M54)</f>
+      <c r="M59" s="7">
+        <f>1000*M55/(M56+M57)</f>
         <v>4.7872340425531918</v>
       </c>
-      <c r="N56" t="s">
+      <c r="N59" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I57">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I60">
         <v>1250</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J60" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I58" s="2">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I61" s="2">
         <v>0.75</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J61" t="s">
         <v>8</v>
       </c>
-      <c r="M58">
+      <c r="M61">
         <v>2.4500000000000002</v>
       </c>
-      <c r="N58" t="s">
+      <c r="N61" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I59" s="1">
-        <f>+I57*I58/I56</f>
-        <v>429.84338173701758</v>
-      </c>
-      <c r="J59" t="s">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I62" s="1">
+        <f>+I60*I61/I59</f>
+        <v>457.77254933467793</v>
+      </c>
+      <c r="J62" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I60" s="7">
-        <f>+I59/365</f>
-        <v>1.1776531006493631</v>
-      </c>
-      <c r="J60" t="s">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I63" s="7">
+        <f>+I62/365</f>
+        <v>1.2541713680402136</v>
+      </c>
+      <c r="J63" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I67">
+    <row r="70" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I70">
         <v>4.2</v>
       </c>
-      <c r="J67" t="s">
+      <c r="J70" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I68" s="7">
-        <f>+I7*I67</f>
-        <v>11.245125991489363</v>
-      </c>
-      <c r="J68" t="s">
+    <row r="71" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I71" s="7">
+        <f>+I8*I70</f>
+        <v>6.933635591489363</v>
+      </c>
+      <c r="J71" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I69">
+    <row r="72" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I72">
         <v>8</v>
       </c>
-      <c r="J69" t="s">
+      <c r="J72" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I70" s="7">
-        <f>+I68/I69</f>
-        <v>1.4056407489361704</v>
-      </c>
-      <c r="J70" t="s">
+    <row r="73" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I73" s="7">
+        <f>+I71/I72</f>
+        <v>0.86670444893617038</v>
+      </c>
+      <c r="J73" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C84">
-        <v>2555</v>
-      </c>
-      <c r="D84" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C85">
-        <f>+M53/(M53+M54)</f>
-        <v>0.5</v>
-      </c>
-      <c r="D85" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C86">
-        <f>+C84*C83/C85</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>2555</v>
+      </c>
+      <c r="D87" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <f>+M56/(M56+M57)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D88" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <f>+C87*C86/C88</f>
         <v>5110</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D89" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor cleanup, report more parameetrs
</commit_message>
<xml_diff>
--- a/hardware/Power consumption.xlsx
+++ b/hardware/Power consumption.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernd\Documents\Documents\Projects\HomeAutomation\MySoilSensorESP32\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC795244-4F71-47F9-91FA-4B0E885DADF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DFD72C-9C86-4768-968E-FB6C2E52AB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3423" yWindow="3423" windowWidth="22212" windowHeight="14373" xr2:uid="{C5D42818-61E1-41CB-B279-D40255C4939D}"/>
+    <workbookView xWindow="21233" yWindow="3682" windowWidth="24209" windowHeight="14372" xr2:uid="{C5D42818-61E1-41CB-B279-D40255C4939D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="45">
   <si>
     <t>State</t>
   </si>
@@ -336,6 +336,15 @@
   </si>
   <si>
     <t>ESP32c3, 2x AAA</t>
+  </si>
+  <si>
+    <t>charge [mC]</t>
+  </si>
+  <si>
+    <t>mC per wake, measured</t>
+  </si>
+  <si>
+    <t>mC per wake, calculated</t>
   </si>
 </sst>
 </file>
@@ -746,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F643F03A-9FCE-4307-81DB-66D7872B7CDB}">
   <dimension ref="B1:R90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1049,6 +1058,9 @@
       <c r="J15" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="K15" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1058,7 +1070,7 @@
         <v>300</v>
       </c>
       <c r="E16">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G16">
         <v>24</v>
@@ -1069,11 +1081,15 @@
       </c>
       <c r="I16" s="4">
         <f>+(E16+F16/1000)*H16/3600</f>
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="J16">
         <f>+E16*H16/(24*60*60)</f>
-        <v>4.1666666666666666E-3</v>
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="K16">
+        <f>+D16*E16/1000</f>
+        <v>9</v>
       </c>
       <c r="M16">
         <v>3</v>
@@ -1081,13 +1097,19 @@
       <c r="N16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>87</v>
+      </c>
+      <c r="R16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>34</v>
       </c>
       <c r="D17">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E17">
         <v>130</v>
@@ -1097,18 +1119,29 @@
       </c>
       <c r="H17">
         <f>+G17*D17/1000</f>
-        <v>7.2</v>
+        <v>14.4</v>
       </c>
       <c r="I17" s="4">
         <f>+(E17+F17/1000)*H17/3600</f>
-        <v>0.26</v>
+        <v>0.52</v>
       </c>
       <c r="J17">
         <f>+E17*H17/(24*60*60)</f>
-        <v>1.0833333333333334E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+        <v>2.1666666666666667E-2</v>
+      </c>
+      <c r="K17">
+        <f>+D17*E17/1000</f>
+        <v>78</v>
+      </c>
+      <c r="Q17">
+        <f>SUM(K16:K17)</f>
+        <v>87</v>
+      </c>
+      <c r="R17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>25</v>
       </c>
@@ -1135,12 +1168,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="F19">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H19">
         <f>24*60*60-SUM(H16:H16)</f>
@@ -1148,7 +1181,7 @@
       </c>
       <c r="I19" s="4">
         <f>+(E19+F19/1000)*H19/3600</f>
-        <v>0.33597199999999999</v>
+        <v>0.11999</v>
       </c>
       <c r="J19" s="6">
         <f>+E19*H19/(24*60*60)</f>
@@ -1161,7 +1194,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>12</v>
       </c>
@@ -1185,10 +1218,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I21" s="5">
         <f>SUM(I16:I20)</f>
-        <v>1.6125677446808511</v>
+        <v>1.6165857446808514</v>
       </c>
       <c r="J21" t="s">
         <v>6</v>
@@ -1201,7 +1234,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I22">
         <v>1250</v>
       </c>
@@ -1209,7 +1242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I23" s="2">
         <v>0.75</v>
       </c>
@@ -1223,30 +1256,30 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I24" s="1">
         <f>+I22*I23/I21</f>
-        <v>581.3709241626583</v>
+        <v>579.92593531441946</v>
       </c>
       <c r="J24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I25" s="7">
         <f>+I24/365</f>
-        <v>1.5927970525004338</v>
+        <v>1.588838178943615</v>
       </c>
       <c r="J25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>0</v>
       </c>
@@ -1275,7 +1308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>40</v>
       </c>
@@ -1283,7 +1316,7 @@
         <v>300</v>
       </c>
       <c r="E29">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G29">
         <v>24</v>
@@ -1294,11 +1327,11 @@
       </c>
       <c r="I29" s="4">
         <f>+(E29+F29/1000)*H29/3600</f>
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="J29">
         <f>+E29*H29/(24*60*60)</f>
-        <v>4.1666666666666666E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="M29">
         <v>3</v>
@@ -1307,12 +1340,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>34</v>
       </c>
       <c r="D30">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E30">
         <v>130</v>
@@ -1322,18 +1355,18 @@
       </c>
       <c r="H30">
         <f>+G30*D30/1000</f>
-        <v>7.2</v>
+        <v>14.4</v>
       </c>
       <c r="I30" s="4">
         <f>+(E30+F30/1000)*H30/3600</f>
-        <v>0.26</v>
+        <v>0.52</v>
       </c>
       <c r="J30">
         <f>+E30*H30/(24*60*60)</f>
-        <v>1.0833333333333334E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+        <v>2.1666666666666667E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>25</v>
       </c>
@@ -1360,12 +1393,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>5</v>
       </c>
       <c r="F32">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H32">
         <f>24*60*60-SUM(H29:H29)</f>
@@ -1373,7 +1406,7 @@
       </c>
       <c r="I32" s="4">
         <f>+(E32+F32/1000)*H32/3600</f>
-        <v>0.33597199999999999</v>
+        <v>0.11999</v>
       </c>
       <c r="J32" s="6">
         <f>+E32*H32/(24*60*60)</f>
@@ -1413,7 +1446,7 @@
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I34" s="5">
         <f>SUM(I29:I33)</f>
-        <v>2.6925677446808507</v>
+        <v>2.696585744680851</v>
       </c>
       <c r="J34" t="s">
         <v>6</v>
@@ -1451,7 +1484,7 @@
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I37" s="1">
         <f>+I35*I36/I34</f>
-        <v>804.99367352293416</v>
+        <v>803.79420690608526</v>
       </c>
       <c r="J37" t="s">
         <v>7</v>
@@ -1460,7 +1493,7 @@
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I38" s="7">
         <f>+I37/365</f>
-        <v>2.2054621192409156</v>
+        <v>2.2021759093317406</v>
       </c>
       <c r="J38" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
various cleanup and refactoring
</commit_message>
<xml_diff>
--- a/hardware/Power consumption.xlsx
+++ b/hardware/Power consumption.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernd\Documents\Documents\Projects\HomeAutomation\MySoilSensorESP32\hardware\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DFD72C-9C86-4768-968E-FB6C2E52AB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="21233" yWindow="3682" windowWidth="24209" windowHeight="14372" xr2:uid="{C5D42818-61E1-41CB-B279-D40255C4939D}"/>
+    <workbookView xWindow="21233" yWindow="3682" windowWidth="24208" windowHeight="14373"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +19,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>bernd</author>
   </authors>
   <commentList>
-    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{B44EB038-C6AC-4BFE-A03F-74DCCADF4C25}">
+    <comment ref="F7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{DA0235EB-4C0C-4C97-9A69-E73950A3A9FB}">
+    <comment ref="F20" authorId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{0B140197-1585-4AB9-8FEA-AE98B2B1082A}">
+    <comment ref="F33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -135,42 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{A65A902B-EC15-49E4-A37E-7CE8D0607B04}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>bernd:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Alkaline AA: 
-   80µA  
-   2890 mAh
-Alkaline AAA: 
-   35µA 
-   1250 mAh
-CR2032: 
-   210 mAh
-   3µA
-Li-Ion: 
-   4400 mAh
-   600µA</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F59" authorId="0" shapeId="0" xr:uid="{AC994FE4-F3AB-4E34-95F5-BFCD19FB6CE7}">
+    <comment ref="F46" authorId="0">
       <text>
         <r>
           <rPr>
@@ -210,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="44">
   <si>
     <t>State</t>
   </si>
@@ -290,15 +249,6 @@
     <t>battery monitor</t>
   </si>
   <si>
-    <t>counts</t>
-  </si>
-  <si>
-    <t>scale</t>
-  </si>
-  <si>
-    <t>mV</t>
-  </si>
-  <si>
     <t>ESP32-WROOM, 3x AAA 4.5V</t>
   </si>
   <si>
@@ -335,9 +285,6 @@
     <t>Active, Wifi off</t>
   </si>
   <si>
-    <t>ESP32c3, 2x AAA</t>
-  </si>
-  <si>
     <t>charge [mC]</t>
   </si>
   <si>
@@ -345,12 +292,21 @@
   </si>
   <si>
     <t>mC per wake, calculated</t>
+  </si>
+  <si>
+    <t>First cycle, fresh connect to Wifi:</t>
+  </si>
+  <si>
+    <t>ms WiFi ON</t>
+  </si>
+  <si>
+    <t>ms WiFi OFF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -499,7 +455,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -551,7 +507,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -745,18 +701,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F643F03A-9FCE-4307-81DB-66D7872B7CDB}">
-  <dimension ref="B1:R90"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -770,7 +726,7 @@
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="2:18" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
@@ -804,28 +760,28 @@
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E3">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G3">
         <v>24</v>
       </c>
       <c r="H3">
         <f>+G3*D3/1000</f>
-        <v>7.2</v>
+        <v>9.6</v>
       </c>
       <c r="I3" s="4">
         <f>+(E3+F3/1000)*H3/3600</f>
-        <v>0.1</v>
+        <v>0.10933333333333332</v>
       </c>
       <c r="J3">
         <f>+E3*H3/(24*60*60)</f>
-        <v>4.1666666666666666E-3</v>
+        <v>4.5555555555555549E-3</v>
       </c>
       <c r="M3">
         <v>4.5</v>
@@ -837,39 +793,39 @@
         <v>3</v>
       </c>
       <c r="R3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E4">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="G4">
         <v>24</v>
       </c>
       <c r="H4">
         <f>+G4*D4/1000</f>
-        <v>7.2</v>
+        <v>14.4</v>
       </c>
       <c r="I4" s="4">
         <f>+(E4+F4/1000)*H4/3600</f>
-        <v>0.26</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="J4">
         <f>+E4*H4/(24*60*60)</f>
-        <v>1.0833333333333334E-2</v>
+        <v>2.3333333333333334E-2</v>
       </c>
       <c r="Q4">
         <v>200</v>
       </c>
       <c r="R4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
@@ -903,7 +859,7 @@
         <v>15</v>
       </c>
       <c r="R5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -915,11 +871,11 @@
       </c>
       <c r="H6">
         <f>24*60*60-SUM(H3:H3)</f>
-        <v>86392.8</v>
+        <v>86390.399999999994</v>
       </c>
       <c r="I6" s="4">
         <f>+(E6+F6/1000)*H6/3600</f>
-        <v>0.33597199999999999</v>
+        <v>0.33596266666666669</v>
       </c>
       <c r="J6" s="6">
         <f>+E6*H6/(24*60*60)</f>
@@ -935,7 +891,7 @@
         <v>4</v>
       </c>
       <c r="R6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
@@ -966,13 +922,13 @@
         <v>60</v>
       </c>
       <c r="R7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I8" s="5">
         <f>SUM(I3:I7)</f>
-        <v>1.6508656170212768</v>
+        <v>1.9601896170212767</v>
       </c>
       <c r="J8" t="s">
         <v>6</v>
@@ -1010,7 +966,7 @@
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I11" s="1">
         <f>+I9*I10/I8</f>
-        <v>567.88389698948902</v>
+        <v>478.27005706959829</v>
       </c>
       <c r="J11" t="s">
         <v>7</v>
@@ -1019,7 +975,7 @@
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I12" s="7">
         <f>+I11/365</f>
-        <v>1.5558462931218877</v>
+        <v>1.3103289234783515</v>
       </c>
       <c r="J12" t="s">
         <v>11</v>
@@ -1027,7 +983,7 @@
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:18" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
@@ -1059,37 +1015,37 @@
         <v>10</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D16">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G16">
         <v>24</v>
       </c>
       <c r="H16">
         <f>+G16*D16/1000</f>
-        <v>7.2</v>
+        <v>9.6</v>
       </c>
       <c r="I16" s="4">
         <f>+(E16+F16/1000)*H16/3600</f>
-        <v>0.06</v>
+        <v>0.10933333333333332</v>
       </c>
       <c r="J16">
         <f>+E16*H16/(24*60*60)</f>
-        <v>2.5000000000000001E-3</v>
+        <v>4.5555555555555549E-3</v>
       </c>
       <c r="K16">
         <f>+D16*E16/1000</f>
-        <v>9</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="M16">
         <v>3</v>
@@ -1101,18 +1057,18 @@
         <v>87</v>
       </c>
       <c r="R16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D17">
         <v>600</v>
       </c>
       <c r="E17">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="G17">
         <v>24</v>
@@ -1123,22 +1079,22 @@
       </c>
       <c r="I17" s="4">
         <f>+(E17+F17/1000)*H17/3600</f>
-        <v>0.52</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="J17">
         <f>+E17*H17/(24*60*60)</f>
-        <v>2.1666666666666667E-2</v>
+        <v>2.3333333333333334E-2</v>
       </c>
       <c r="K17">
         <f>+D17*E17/1000</f>
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="Q17">
         <f>SUM(K16:K17)</f>
-        <v>87</v>
+        <v>100.4</v>
       </c>
       <c r="R17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
@@ -1177,11 +1133,11 @@
       </c>
       <c r="H19">
         <f>24*60*60-SUM(H16:H16)</f>
-        <v>86392.8</v>
+        <v>86390.399999999994</v>
       </c>
       <c r="I19" s="4">
         <f>+(E19+F19/1000)*H19/3600</f>
-        <v>0.11999</v>
+        <v>0.11998666666666667</v>
       </c>
       <c r="J19" s="6">
         <f>+E19*H19/(24*60*60)</f>
@@ -1192,6 +1148,9 @@
       </c>
       <c r="N19" t="s">
         <v>17</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
@@ -1217,11 +1176,17 @@
       <c r="N20" t="s">
         <v>18</v>
       </c>
+      <c r="Q20">
+        <v>2200</v>
+      </c>
+      <c r="R20" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I21" s="5">
         <f>SUM(I16:I20)</f>
-        <v>1.6165857446808514</v>
+        <v>1.7059157446808513</v>
       </c>
       <c r="J21" t="s">
         <v>6</v>
@@ -1233,6 +1198,12 @@
       <c r="N21" t="s">
         <v>19</v>
       </c>
+      <c r="Q21">
+        <v>600</v>
+      </c>
+      <c r="R21" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I22">
@@ -1259,7 +1230,7 @@
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I24" s="1">
         <f>+I22*I23/I21</f>
-        <v>579.92593531441946</v>
+        <v>549.55820820763381</v>
       </c>
       <c r="J24" t="s">
         <v>7</v>
@@ -1268,7 +1239,7 @@
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I25" s="7">
         <f>+I24/365</f>
-        <v>1.588838178943615</v>
+        <v>1.5056389265962571</v>
       </c>
       <c r="J25" t="s">
         <v>11</v>
@@ -1276,7 +1247,7 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="2:18" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
@@ -1310,28 +1281,28 @@
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D29">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E29">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G29">
         <v>24</v>
       </c>
       <c r="H29">
         <f>+G29*D29/1000</f>
-        <v>7.2</v>
+        <v>9.6</v>
       </c>
       <c r="I29" s="4">
         <f>+(E29+F29/1000)*H29/3600</f>
-        <v>0.06</v>
+        <v>0.10933333333333332</v>
       </c>
       <c r="J29">
         <f>+E29*H29/(24*60*60)</f>
-        <v>2.5000000000000001E-3</v>
+        <v>4.5555555555555549E-3</v>
       </c>
       <c r="M29">
         <v>3</v>
@@ -1342,13 +1313,13 @@
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D30">
         <v>600</v>
       </c>
       <c r="E30">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="G30">
         <v>24</v>
@@ -1359,11 +1330,11 @@
       </c>
       <c r="I30" s="4">
         <f>+(E30+F30/1000)*H30/3600</f>
-        <v>0.52</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="J30">
         <f>+E30*H30/(24*60*60)</f>
-        <v>2.1666666666666667E-2</v>
+        <v>2.3333333333333334E-2</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
@@ -1402,11 +1373,11 @@
       </c>
       <c r="H32">
         <f>24*60*60-SUM(H29:H29)</f>
-        <v>86392.8</v>
+        <v>86390.399999999994</v>
       </c>
       <c r="I32" s="4">
         <f>+(E32+F32/1000)*H32/3600</f>
-        <v>0.11999</v>
+        <v>0.11998666666666667</v>
       </c>
       <c r="J32" s="6">
         <f>+E32*H32/(24*60*60)</f>
@@ -1446,7 +1417,7 @@
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I34" s="5">
         <f>SUM(I29:I33)</f>
-        <v>2.696585744680851</v>
+        <v>2.7859157446808509</v>
       </c>
       <c r="J34" t="s">
         <v>6</v>
@@ -1484,7 +1455,7 @@
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I37" s="1">
         <f>+I35*I36/I34</f>
-        <v>803.79420690608526</v>
+        <v>778.02065770955494</v>
       </c>
       <c r="J37" t="s">
         <v>7</v>
@@ -1493,7 +1464,7 @@
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I38" s="7">
         <f>+I37/365</f>
-        <v>2.2021759093317406</v>
+        <v>2.1315634457796024</v>
       </c>
       <c r="J38" t="s">
         <v>11</v>
@@ -1501,10 +1472,10 @@
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
@@ -1538,28 +1509,28 @@
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D42">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E42">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G42">
         <v>24</v>
       </c>
       <c r="H42">
         <f>+G42*D42/1000</f>
-        <v>7.2</v>
+        <v>9.6</v>
       </c>
       <c r="I42" s="4">
         <f>+(E42+F42/1000)*H42/3600</f>
-        <v>0.1</v>
+        <v>0.10933333333333332</v>
       </c>
       <c r="J42">
         <f>+E42*H42/(24*60*60)</f>
-        <v>4.1666666666666666E-3</v>
+        <v>4.5555555555555549E-3</v>
       </c>
       <c r="M42">
         <v>3</v>
@@ -1570,28 +1541,28 @@
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D43">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E43">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="G43">
         <v>24</v>
       </c>
       <c r="H43">
         <f>+G43*D43/1000</f>
-        <v>7.2</v>
+        <v>14.4</v>
       </c>
       <c r="I43" s="4">
         <f>+(E43+F43/1000)*H43/3600</f>
-        <v>0.26</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="J43">
         <f>+E43*H43/(24*60*60)</f>
-        <v>1.0833333333333334E-2</v>
+        <v>2.3333333333333334E-2</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
@@ -1630,11 +1601,11 @@
       </c>
       <c r="H45">
         <f>24*60*60-SUM(H42:H42)</f>
-        <v>86392.8</v>
+        <v>86390.399999999994</v>
       </c>
       <c r="I45" s="4">
         <f>+(E45+F45/1000)*H45/3600</f>
-        <v>0.33597199999999999</v>
+        <v>0.33596266666666669</v>
       </c>
       <c r="J45" s="6">
         <f>+E45*H45/(24*60*60)</f>
@@ -1674,7 +1645,7 @@
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I47" s="5">
         <f>SUM(I42:I46)</f>
-        <v>0.84456774468085094</v>
+        <v>1.1538917446808512</v>
       </c>
       <c r="J47" t="s">
         <v>6</v>
@@ -1695,7 +1666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="9:14" x14ac:dyDescent="0.25">
       <c r="I49" s="2">
         <v>0.75</v>
       </c>
@@ -1709,312 +1680,56 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:14" x14ac:dyDescent="0.25">
       <c r="I50" s="1">
         <f>+I48*I49/I47</f>
-        <v>195.36621075003396</v>
+        <v>142.99434999912967</v>
       </c>
       <c r="J50" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="9:14" x14ac:dyDescent="0.25">
       <c r="I51" s="7">
         <f>+I50/365</f>
-        <v>0.53524989246584642</v>
+        <v>0.39176534246336897</v>
       </c>
       <c r="J51" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B53" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" s="3" customFormat="1" ht="28.55" x14ac:dyDescent="0.25">
-      <c r="B54" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>40</v>
-      </c>
-      <c r="D55">
-        <v>200</v>
-      </c>
-      <c r="E55">
+    <row r="56" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>4.2</v>
+      </c>
+      <c r="J56" t="s">
         <v>20</v>
       </c>
-      <c r="G55">
-        <v>24</v>
-      </c>
-      <c r="H55">
-        <f>+G55*D55/1000</f>
-        <v>4.8</v>
-      </c>
-      <c r="I55" s="4">
-        <f>+(E55+F55/1000)*H55/3600</f>
-        <v>2.6666666666666668E-2</v>
-      </c>
-      <c r="J55">
-        <f>+E55*H55/(24*60*60)</f>
-        <v>1.1111111111111111E-3</v>
-      </c>
-      <c r="M55">
-        <v>4.5</v>
-      </c>
-      <c r="N55" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>34</v>
-      </c>
-      <c r="D56">
-        <v>400</v>
-      </c>
-      <c r="E56">
-        <v>80</v>
-      </c>
-      <c r="G56">
-        <v>24</v>
-      </c>
-      <c r="H56">
-        <f>+G56*D56/1000</f>
-        <v>9.6</v>
-      </c>
-      <c r="I56" s="4">
-        <f>+(E56+F56/1000)*H56/3600</f>
-        <v>0.21333333333333335</v>
-      </c>
-      <c r="J56">
-        <f>+E56*H56/(24*60*60)</f>
-        <v>8.8888888888888889E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>25</v>
-      </c>
-      <c r="F57" s="7">
-        <f>+M60</f>
-        <v>4.7872340425531918</v>
-      </c>
-      <c r="H57">
-        <f>24*60*60</f>
-        <v>86400</v>
-      </c>
-      <c r="I57" s="4">
-        <f>+(E57+F57/1000)*H57/3600</f>
-        <v>0.1148936170212766</v>
-      </c>
-      <c r="J57">
-        <f>+E57*H57/(24*60*60)</f>
-        <v>0</v>
-      </c>
-      <c r="M57">
-        <v>470</v>
-      </c>
-      <c r="N57" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>5</v>
-      </c>
-      <c r="F58">
-        <v>40</v>
-      </c>
-      <c r="H58">
-        <f>24*60*60-SUM(H55:H55)</f>
-        <v>86395.199999999997</v>
-      </c>
-      <c r="I58" s="4">
-        <f>+(E58+F58/1000)*H58/3600</f>
-        <v>0.95994666666666661</v>
-      </c>
-      <c r="J58" s="6">
-        <f>+E58*H58/(24*60*60)</f>
-        <v>0</v>
-      </c>
-      <c r="M58">
-        <v>470</v>
-      </c>
-      <c r="N58" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59">
-        <v>35</v>
-      </c>
-      <c r="H59">
-        <f>24*60*60</f>
-        <v>86400</v>
-      </c>
-      <c r="I59" s="4">
-        <f>+(E59+F59/1000)*H59/3600</f>
-        <v>0.84000000000000008</v>
-      </c>
-      <c r="J59" s="6"/>
-      <c r="M59" s="4">
-        <f>+M55*M57/(M57+M58)</f>
-        <v>2.25</v>
-      </c>
-      <c r="N59" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I60" s="5">
-        <f>SUM(I55:I59)</f>
-        <v>2.1548402836879434</v>
-      </c>
-      <c r="J60" t="s">
-        <v>6</v>
-      </c>
-      <c r="M60" s="7">
-        <f>1000*M55/(M57+M58)</f>
-        <v>4.7872340425531918</v>
-      </c>
-      <c r="N60" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I61">
-        <v>1250</v>
-      </c>
-      <c r="J61" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I62" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="J62" t="s">
+    </row>
+    <row r="57" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I57" s="7">
+        <f>+I8*I56</f>
+        <v>8.2327963914893623</v>
+      </c>
+      <c r="J57" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I58">
         <v>8</v>
       </c>
-      <c r="M62">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="N62" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I63" s="1">
-        <f>+I61*I62/I60</f>
-        <v>435.06704747300216</v>
-      </c>
-      <c r="J63" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I64" s="7">
-        <f>+I63/365</f>
-        <v>1.1919645136246635</v>
-      </c>
-      <c r="J64" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I71">
-        <v>4.2</v>
-      </c>
-      <c r="J71" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="72" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I72" s="7">
-        <f>+I8*I71</f>
-        <v>6.933635591489363</v>
-      </c>
-      <c r="J72" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="73" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I73">
-        <v>8</v>
-      </c>
-      <c r="J73" t="s">
+      <c r="J58" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="74" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I74" s="7">
-        <f>+I72/I73</f>
-        <v>0.86670444893617038</v>
-      </c>
-      <c r="J74" t="s">
+    <row r="59" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I59" s="7">
+        <f>+I57/I58</f>
+        <v>1.0290995489361703</v>
+      </c>
+      <c r="J59" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C88">
-        <v>2555</v>
-      </c>
-      <c r="D88" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C89">
-        <f>+M57/(M57+M58)</f>
-        <v>0.5</v>
-      </c>
-      <c r="D89" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C90">
-        <f>+C88*C87/C89</f>
-        <v>5110</v>
-      </c>
-      <c r="D90" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>